<commit_message>
Planning Extended - 2877392159 업데이트
</commit_message>
<xml_diff>
--- a/Data/Planning Extended - 2877392159/2877392159.xlsx
+++ b/Data/Planning Extended - 2877392159/2877392159.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Steam\steamapps\common\RimWorld\Mods\RMK\Data\Planning Extended - 2877392159\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bjmi0\Desktop\림월드 번역\Planning Extended - 2877392159\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E191C6EE-90F2-4A3F-AAA1-372ABCBDD16E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2253F30E-917C-47E3-B7AE-8C2969720354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="0" windowWidth="38380" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main_240425" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="454">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="521">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -1303,10 +1303,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">색상 팰럿 </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>MorePlanning 계획 변환</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -1436,6 +1432,268 @@
   </si>
   <si>
     <t>십자선</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>계획 확장</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>계획 확장 모드에서 사용하는 도구들입니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>색상 선택</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>수정</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>덮어쓰기 금지</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>형상 변환</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>작업 1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>작업 2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>저장된 계획을 붙여넣습니다.\n\n키를 사용해 회전하거나 뒤집을 수 있습니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>마지막으로 생성한 계획 작업을 취소합니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>마지막으로 취소한 계획 작업을 다시 실행합니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>파일에서 계획을 불러옵니다.\n\n좌클릭으로 계획 목록을 열 수 있습니다.\n\n우클릭으로 마지막으로 불러온 계획을 빠르게 선택할 수 있습니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>마지막으로 복사한 계획을 파일에 저장합니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>계획 보이기 전환</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>모든 계획의 가시성을 전환합니다.\n\n(0)을 누른 상태로 각 계획을 선택하면 개별로 전환할 수 있습니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>좌클릭으로 불투명도를 설정합니다.\n\n우클릭으로 텍스처 세트를 변경합니다.\n\n(0)을 누른 상태로 각 계획을 선택하면 개별로 전환할 수 있습니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>색상 계획을 선택합니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>기존 계획에서 색상을 가져옵니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>문 형태의 계획을 배치합니다.\n\n우클릭으로 형태를 선택할 수 있습니다.\n\n{0} 키를 눌러 색상을 선택할 수 있습니다.\n\n{1} 키를 눌러 크기를 조절할 수 있습니다.</t>
+  </si>
+  <si>
+    <t>바닥 형태의 계획을 배치합니다.\n\n우클릭으로 형태를 선택할 수 있습니다.\n\n{0} 키를 눌러 색상을 선택할 수 있습니다.\n\n{1} 키를 눌러 크기를 조절할 수 있습니다.</t>
+  </si>
+  <si>
+    <t>구조물 형태의 계획을 배치합니다.\n\n우클릭으로 형태를 선택할 수 있습니다.\n\n{0} 키를 눌러 색상을 선택할 수 있습니다.\n\n{1} 키를 눌러 크기를 조절할 수 있습니다.</t>
+  </si>
+  <si>
+    <t>벽 형태의 계획을 배치합니다.\n\n우클릭으로 형태를 선택할 수 있습니다.\n\n{0} 키를 눌러 색상을 선택할 수 있습니다.\n\n{1} 키를 눌러 크기를 조절할 수 있습니다.</t>
+  </si>
+  <si>
+    <t>이미 존재하는 계획을 채색합니다.\n\n우클릭으로 형태를 선택할 수 있습니다.\n\n{0} 키를 눌러 색상을 선택할 수 있습니다.\n\n{1} 키를 눌러 크기를 조절할 수 있습니다.</t>
+  </si>
+  <si>
+    <t>계획을 제거합니다.</t>
+  </si>
+  <si>
+    <t>선택한 영역의 계획을 복사합니다.</t>
+  </si>
+  <si>
+    <t>선택한 영역의 계획을 잘라내 복사합니다.</t>
+  </si>
+  <si>
+    <t>계획을 찾을 수 없습니다.</t>
+  </si>
+  <si>
+    <t>계획이 복사되었습니다.</t>
+  </si>
+  <si>
+    <t>계획을 삭제합니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>계획을 {0}(으)로 저장합니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>{0} {1} 계획을 삭제합니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>문</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>바닥</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>구조물</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>벽</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>모드</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>복사</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>잘라내기</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>건너뛰기</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>교체</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>잘라내기로 전환</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>되돌리기-다시 실행</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>되돌리기-다시 실행 기능을 사용하고 버튼이 표시될지 여부를 결정합니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>활성화하면 계획 잘라내기 버튼이 표시됩니다. 비활성화하면 보이지 않습니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>활성화하면 계획 보이기 버튼이 표시됩니다. 비활성화하면 보이지 않습니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>보기 설정 버튼 표시</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>활성화하면 보기 설정 버튼이 표시됩니다. 비활성화하면 보이지 않습니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>활성화하면 건설을 완료한 후에도 계획이 유지됩니다. 비활성화하면 제거됩니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>활성화하면 컨트롤 키를 눌러 색상 목록을 표시할 수 있습니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>컨트롤 키로 색상 띄우기</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>교체 대신 건너뛰기를 기본값으로 사용</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>활성화하면 기본적으로 계획을 건너뜁니다. 비활성화하면 교체를 기본값으로 사용합니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>계획 표시</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>계획의 표시 여부를 결정합니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>{0} 개수</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>넓이</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>없음</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>북</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>동</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>남</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>남서</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>서</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>북서</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>북동</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>남동</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>대각</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>북서 대각</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>북동 대각</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1800,8 +2058,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
-      <selection activeCell="F58" sqref="F58"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F121" sqref="F121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -1866,6 +2124,9 @@
       <c r="E3" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="F3" s="1" t="s">
+        <v>453</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
@@ -1880,6 +2141,9 @@
       <c r="E4" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="F4" s="1" t="s">
+        <v>454</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
@@ -1894,6 +2158,9 @@
       <c r="E5" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="F5" s="1" t="s">
+        <v>466</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
@@ -1908,6 +2175,9 @@
       <c r="E6" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="F6" s="1" t="s">
+        <v>455</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
@@ -1922,6 +2192,9 @@
       <c r="E7" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="F7" s="1" t="s">
+        <v>456</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
@@ -1936,6 +2209,9 @@
       <c r="E8" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="F8" s="1" t="s">
+        <v>457</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
@@ -1950,6 +2226,9 @@
       <c r="E9" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="F9" s="1" t="s">
+        <v>411</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
@@ -1964,6 +2243,9 @@
       <c r="E10" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="F10" s="1" t="s">
+        <v>412</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
@@ -1978,6 +2260,9 @@
       <c r="E11" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="F11" s="1" t="s">
+        <v>413</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
@@ -1992,6 +2277,9 @@
       <c r="E12" s="1" t="s">
         <v>40</v>
       </c>
+      <c r="F12" s="1" t="s">
+        <v>414</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
@@ -2006,6 +2294,9 @@
       <c r="E13" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="F13" s="1" t="s">
+        <v>458</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
@@ -2020,6 +2311,9 @@
       <c r="E14" s="1" t="s">
         <v>46</v>
       </c>
+      <c r="F14" s="1" t="s">
+        <v>459</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
@@ -2034,6 +2328,9 @@
       <c r="E15" s="1" t="s">
         <v>49</v>
       </c>
+      <c r="F15" s="1" t="s">
+        <v>460</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
@@ -2048,6 +2345,9 @@
       <c r="E16" s="1" t="s">
         <v>52</v>
       </c>
+      <c r="F16" s="1" t="s">
+        <v>404</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
@@ -2062,6 +2362,9 @@
       <c r="E17" s="1" t="s">
         <v>55</v>
       </c>
+      <c r="F17" s="1" t="s">
+        <v>405</v>
+      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
@@ -2077,7 +2380,7 @@
         <v>59</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
@@ -2094,7 +2397,7 @@
         <v>62</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
@@ -2127,6 +2430,9 @@
       <c r="E21" s="1" t="s">
         <v>68</v>
       </c>
+      <c r="F21" s="1" t="s">
+        <v>471</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
@@ -2158,6 +2464,9 @@
       <c r="E23" s="1" t="s">
         <v>74</v>
       </c>
+      <c r="F23" s="1" t="s">
+        <v>472</v>
+      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
@@ -2189,6 +2498,9 @@
       <c r="E25" s="1" t="s">
         <v>80</v>
       </c>
+      <c r="F25" s="1" t="s">
+        <v>473</v>
+      </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
@@ -2220,6 +2532,9 @@
       <c r="E27" s="1" t="s">
         <v>86</v>
       </c>
+      <c r="F27" s="1" t="s">
+        <v>474</v>
+      </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
@@ -2251,6 +2566,9 @@
       <c r="E29" s="1" t="s">
         <v>92</v>
       </c>
+      <c r="F29" s="1" t="s">
+        <v>475</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
@@ -2282,6 +2600,9 @@
       <c r="E31" s="1" t="s">
         <v>98</v>
       </c>
+      <c r="F31" s="1" t="s">
+        <v>476</v>
+      </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
@@ -2313,6 +2634,9 @@
       <c r="E33" s="1" t="s">
         <v>104</v>
       </c>
+      <c r="F33" s="1" t="s">
+        <v>477</v>
+      </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
@@ -2344,6 +2668,9 @@
       <c r="E35" s="1" t="s">
         <v>110</v>
       </c>
+      <c r="F35" s="1" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
@@ -2375,6 +2702,9 @@
       <c r="E37" s="1" t="s">
         <v>116</v>
       </c>
+      <c r="F37" s="1" t="s">
+        <v>461</v>
+      </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
@@ -2406,6 +2736,9 @@
       <c r="E39" s="1" t="s">
         <v>122</v>
       </c>
+      <c r="F39" s="1" t="s">
+        <v>462</v>
+      </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
@@ -2437,6 +2770,9 @@
       <c r="E41" s="1" t="s">
         <v>128</v>
       </c>
+      <c r="F41" s="1" t="s">
+        <v>463</v>
+      </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42" s="1" t="s">
@@ -2468,6 +2804,9 @@
       <c r="E43" s="1" t="s">
         <v>134</v>
       </c>
+      <c r="F43" s="1" t="s">
+        <v>464</v>
+      </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
@@ -2499,6 +2838,9 @@
       <c r="E45" s="1" t="s">
         <v>140</v>
       </c>
+      <c r="F45" s="1" t="s">
+        <v>465</v>
+      </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46" s="1" t="s">
@@ -2530,6 +2872,9 @@
       <c r="E47" s="1" t="s">
         <v>146</v>
       </c>
+      <c r="F47" s="1" t="s">
+        <v>467</v>
+      </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A48" s="1" t="s">
@@ -2548,7 +2893,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A49" s="1" t="s">
         <v>150</v>
       </c>
@@ -2561,8 +2906,11 @@
       <c r="E49" s="1" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F49" s="1" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A50" s="1" t="s">
         <v>153</v>
       </c>
@@ -2575,8 +2923,11 @@
       <c r="E50" s="1" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F50" s="1" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A51" s="1" t="s">
         <v>156</v>
       </c>
@@ -2589,8 +2940,11 @@
       <c r="E51" s="1" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F51" s="1" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A52" s="1" t="s">
         <v>159</v>
       </c>
@@ -2603,8 +2957,11 @@
       <c r="E52" s="1" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F52" s="1" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A53" s="1" t="s">
         <v>162</v>
       </c>
@@ -2617,8 +2974,11 @@
       <c r="E53" s="1" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F53" s="1" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A54" s="1" t="s">
         <v>165</v>
       </c>
@@ -2631,8 +2991,11 @@
       <c r="E54" s="1" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F54" s="1" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A55" s="1" t="s">
         <v>168</v>
       </c>
@@ -2645,8 +3008,11 @@
       <c r="E55" s="1" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F55" s="1" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A56" s="1" t="s">
         <v>171</v>
       </c>
@@ -2659,8 +3025,11 @@
       <c r="E56" s="1" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F56" s="1" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A57" s="1" t="s">
         <v>174</v>
       </c>
@@ -2673,8 +3042,11 @@
       <c r="E57" s="1" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F57" s="1" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A58" s="1" t="s">
         <v>177</v>
       </c>
@@ -2687,8 +3059,11 @@
       <c r="E58" s="1" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F58" s="1" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A59" s="1" t="s">
         <v>180</v>
       </c>
@@ -2701,8 +3076,11 @@
       <c r="E59" s="1" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F59" s="1" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A60" s="1" t="s">
         <v>183</v>
       </c>
@@ -2715,8 +3093,11 @@
       <c r="E60" s="1" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F60" s="1" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A61" s="1" t="s">
         <v>186</v>
       </c>
@@ -2729,8 +3110,11 @@
       <c r="E61" s="1" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F61" s="1" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A62" s="1" t="s">
         <v>189</v>
       </c>
@@ -2743,8 +3127,11 @@
       <c r="E62" s="1" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F62" s="1" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A63" s="1" t="s">
         <v>192</v>
       </c>
@@ -2757,8 +3144,11 @@
       <c r="E63" s="1" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F63" s="1" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A64" s="1" t="s">
         <v>195</v>
       </c>
@@ -2770,6 +3160,9 @@
       </c>
       <c r="E64" s="1" t="s">
         <v>197</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.45">
@@ -2785,6 +3178,9 @@
       <c r="E65" s="1" t="s">
         <v>200</v>
       </c>
+      <c r="F65" s="1" t="s">
+        <v>492</v>
+      </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A66" s="1" t="s">
@@ -2799,6 +3195,9 @@
       <c r="E66" s="1" t="s">
         <v>203</v>
       </c>
+      <c r="F66" s="1" t="s">
+        <v>493</v>
+      </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A67" s="1" t="s">
@@ -2813,6 +3212,9 @@
       <c r="E67" s="1" t="s">
         <v>206</v>
       </c>
+      <c r="F67" s="1" t="s">
+        <v>494</v>
+      </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A68" s="1" t="s">
@@ -2844,6 +3246,9 @@
       <c r="E69" s="1" t="s">
         <v>212</v>
       </c>
+      <c r="F69" s="1" t="s">
+        <v>495</v>
+      </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A70" s="1" t="s">
@@ -2892,6 +3297,9 @@
       <c r="E72" s="1" t="s">
         <v>221</v>
       </c>
+      <c r="F72" s="1" t="s">
+        <v>496</v>
+      </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A73" s="1" t="s">
@@ -2923,6 +3331,9 @@
       <c r="E74" s="1" t="s">
         <v>227</v>
       </c>
+      <c r="F74" s="1" t="s">
+        <v>497</v>
+      </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A75" s="1" t="s">
@@ -2937,6 +3348,9 @@
       <c r="E75" s="1" t="s">
         <v>230</v>
       </c>
+      <c r="F75" s="1" t="s">
+        <v>498</v>
+      </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A76" s="1" t="s">
@@ -2951,6 +3365,9 @@
       <c r="E76" s="1" t="s">
         <v>233</v>
       </c>
+      <c r="F76" s="1" t="s">
+        <v>499</v>
+      </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A77" s="1" t="s">
@@ -2982,6 +3399,9 @@
       <c r="E78" s="1" t="s">
         <v>239</v>
       </c>
+      <c r="F78" s="1" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A79" s="1" t="s">
@@ -2997,7 +3417,7 @@
         <v>242</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>420</v>
+        <v>502</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.45">
@@ -3013,6 +3433,9 @@
       <c r="E80" s="1" t="s">
         <v>245</v>
       </c>
+      <c r="F80" s="1" t="s">
+        <v>501</v>
+      </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A81" s="1" t="s">
@@ -3027,6 +3450,9 @@
       <c r="E81" s="1" t="s">
         <v>248</v>
       </c>
+      <c r="F81" s="1" t="s">
+        <v>503</v>
+      </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A82" s="1" t="s">
@@ -3041,6 +3467,9 @@
       <c r="E82" s="1" t="s">
         <v>251</v>
       </c>
+      <c r="F82" s="1" t="s">
+        <v>504</v>
+      </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A83" s="1" t="s">
@@ -3055,6 +3484,9 @@
       <c r="E83" s="1" t="s">
         <v>254</v>
       </c>
+      <c r="F83" s="1" t="s">
+        <v>505</v>
+      </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A84" s="1" t="s">
@@ -3069,6 +3501,9 @@
       <c r="E84" s="1" t="s">
         <v>257</v>
       </c>
+      <c r="F84" s="1" t="s">
+        <v>506</v>
+      </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A85" s="1" t="s">
@@ -3084,7 +3519,7 @@
         <v>260</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.45">
@@ -3101,7 +3536,7 @@
         <v>263</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.45">
@@ -3119,7 +3554,7 @@
         <v>266</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.45">
@@ -3136,7 +3571,7 @@
         <v>269</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.45">
@@ -3153,7 +3588,7 @@
         <v>272</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.45">
@@ -3170,7 +3605,7 @@
         <v>275</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.45">
@@ -3187,7 +3622,7 @@
         <v>278</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.45">
@@ -3204,7 +3639,7 @@
         <v>281</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.45">
@@ -3221,7 +3656,7 @@
         <v>284</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.45">
@@ -3238,7 +3673,7 @@
         <v>287</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.45">
@@ -3256,7 +3691,7 @@
         <v>290</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.45">
@@ -3273,7 +3708,7 @@
         <v>293</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.45">
@@ -3290,7 +3725,7 @@
         <v>296</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.45">
@@ -3307,7 +3742,7 @@
         <v>299</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.45">
@@ -3324,7 +3759,7 @@
         <v>302</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.45">
@@ -3341,7 +3776,7 @@
         <v>305</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.45">
@@ -3358,7 +3793,7 @@
         <v>308</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.45">
@@ -3375,7 +3810,7 @@
         <v>311</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.45">
@@ -3392,7 +3827,7 @@
         <v>314</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.45">
@@ -3409,7 +3844,7 @@
         <v>317</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.45">
@@ -3426,7 +3861,7 @@
         <v>320</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.45">
@@ -3443,7 +3878,7 @@
         <v>323</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.45">
@@ -3460,7 +3895,7 @@
         <v>326</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.45">
@@ -3477,7 +3912,7 @@
         <v>329</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.45">
@@ -3494,7 +3929,7 @@
         <v>332</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.45">
@@ -3511,7 +3946,7 @@
         <v>335</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.45">
@@ -3529,7 +3964,7 @@
         <v>338</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.45">
@@ -3547,7 +3982,7 @@
         <v>341</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.45">
@@ -3563,6 +3998,9 @@
       <c r="E113" s="1" t="s">
         <v>344</v>
       </c>
+      <c r="F113" s="1" t="s">
+        <v>507</v>
+      </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A114" s="1" t="s">
@@ -3578,7 +4016,7 @@
         <v>347</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.45">
@@ -3595,7 +4033,7 @@
         <v>350</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.45">
@@ -3611,6 +4049,9 @@
       <c r="E116" s="1" t="s">
         <v>353</v>
       </c>
+      <c r="F116" s="1" t="s">
+        <v>508</v>
+      </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A117" s="1" t="s">
@@ -3626,7 +4067,7 @@
         <v>356</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.45">
@@ -3642,6 +4083,9 @@
       <c r="E118" s="1" t="s">
         <v>359</v>
       </c>
+      <c r="F118" s="1" t="s">
+        <v>509</v>
+      </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A119" s="1" t="s">
@@ -3656,6 +4100,9 @@
       <c r="E119" s="1" t="s">
         <v>362</v>
       </c>
+      <c r="F119" s="1" t="s">
+        <v>510</v>
+      </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A120" s="1" t="s">
@@ -3670,6 +4117,9 @@
       <c r="E120" s="1" t="s">
         <v>365</v>
       </c>
+      <c r="F120" s="1" t="s">
+        <v>516</v>
+      </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A121" s="1" t="s">
@@ -3684,6 +4134,9 @@
       <c r="E121" s="1" t="s">
         <v>368</v>
       </c>
+      <c r="F121" s="1" t="s">
+        <v>511</v>
+      </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A122" s="1" t="s">
@@ -3698,6 +4151,9 @@
       <c r="E122" s="1" t="s">
         <v>371</v>
       </c>
+      <c r="F122" s="1" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A123" s="1" t="s">
@@ -3712,6 +4168,9 @@
       <c r="E123" s="1" t="s">
         <v>374</v>
       </c>
+      <c r="F123" s="1" t="s">
+        <v>512</v>
+      </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A124" s="1" t="s">
@@ -3726,6 +4185,9 @@
       <c r="E124" s="1" t="s">
         <v>377</v>
       </c>
+      <c r="F124" s="1" t="s">
+        <v>513</v>
+      </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A125" s="1" t="s">
@@ -3740,6 +4202,9 @@
       <c r="E125" s="1" t="s">
         <v>380</v>
       </c>
+      <c r="F125" s="1" t="s">
+        <v>514</v>
+      </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A126" s="1" t="s">
@@ -3754,6 +4219,9 @@
       <c r="E126" s="1" t="s">
         <v>383</v>
       </c>
+      <c r="F126" s="1" t="s">
+        <v>515</v>
+      </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A127" s="1" t="s">
@@ -3769,7 +4237,7 @@
         <v>386</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.45">
@@ -3786,10 +4254,10 @@
         <v>389</v>
       </c>
       <c r="F128" s="1" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.45">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A129" s="1" t="s">
         <v>390</v>
       </c>
@@ -3802,8 +4270,11 @@
       <c r="E129" s="1" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F129" s="1" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A130" s="1" t="s">
         <v>393</v>
       </c>
@@ -3816,8 +4287,11 @@
       <c r="E130" s="1" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F130" s="1" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A131" s="1" t="s">
         <v>396</v>
       </c>
@@ -3829,6 +4303,9 @@
       </c>
       <c r="E131" s="1" t="s">
         <v>398</v>
+      </c>
+      <c r="F131" s="1" t="s">
+        <v>520</v>
       </c>
     </row>
   </sheetData>

</xml_diff>